<commit_message>
commit for the project 7rmart
</commit_message>
<xml_diff>
--- a/7rmart/src/test/resources/TestData.xlsx
+++ b/7rmart/src/test/resources/TestData.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\7mart\7mart\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\7rmart\7rmart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="Manage Contact Page" sheetId="10" r:id="rId2"/>
-    <sheet name="Manage news page" sheetId="2" r:id="rId3"/>
-    <sheet name="Admin Users Page" sheetId="8" r:id="rId4"/>
+    <sheet name="Category Page" sheetId="11" r:id="rId3"/>
+    <sheet name="Manage FooterText Page" sheetId="12" r:id="rId4"/>
+    <sheet name="settings" sheetId="13" r:id="rId5"/>
+    <sheet name="Sub Category page" sheetId="14" r:id="rId6"/>
+    <sheet name="Manage news page" sheetId="2" r:id="rId7"/>
+    <sheet name="Admin Users Page" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>admin</t>
   </si>
@@ -44,9 +48,6 @@
     <t>demo</t>
   </si>
   <si>
-    <t>staff</t>
-  </si>
-  <si>
     <t>3pm</t>
   </si>
   <si>
@@ -65,12 +66,6 @@
     <t>Delivery Charge Limit</t>
   </si>
   <si>
-    <t>gm</t>
-  </si>
-  <si>
-    <t>county road</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -80,20 +75,70 @@
     <t>Value</t>
   </si>
   <si>
+    <t>demotest@gmail.com</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>M &amp; M chocolate</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Menu Name</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Wrist Band</t>
+  </si>
+  <si>
     <t>vivekm</t>
+  </si>
+  <si>
+    <t>Customer grievance</t>
+  </si>
+  <si>
+    <t>SRM Building ,M.G.Road,Kochi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emerald Rd, Marine Drive, Ernakulam, </t>
+  </si>
+  <si>
+    <t>testingdemo@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF474747"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,13 +158,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,10 +465,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,6 +511,65 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8715447910</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -465,44 +577,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1454</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>300</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -510,7 +595,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3">
+        <v>73547896166</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -520,7 +707,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -533,9 +720,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -546,26 +733,20 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>